<commit_message>
Added read data from excel sheet, WebDriverEventListener and fixed login credentials isue
</commit_message>
<xml_diff>
--- a/target/classes/com/crm/qa/testdata/TestData.xlsx
+++ b/target/classes/com/crm/qa/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CRM_Automation\src\main\java\com\crm\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385E0E11-E6EC-4883-9D73-D0FD74B7D199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EFB13B-BE7D-4FBC-ACC9-6D4289143FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -381,7 +381,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>